<commit_message>
Import data use excel
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\MLP\AssetManagement\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\MLP\InventoryATK\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2F2DB-1C04-40D2-9BD5-D01F6B86218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382FD0DB-801F-4E2F-9F1A-B7D4C553488D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
+    <workbookView xWindow="377" yWindow="377" windowWidth="18514" windowHeight="10740" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,48 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Kode Asset Lama</t>
-  </si>
-  <si>
-    <t>Lokasi</t>
-  </si>
-  <si>
-    <t>Kategori</t>
-  </si>
-  <si>
-    <t>Asset Position</t>
-  </si>
-  <si>
-    <t>Jenis</t>
-  </si>
-  <si>
-    <t>Deskripsi</t>
-  </si>
-  <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
-    <t>Tanggal Perolehan</t>
-  </si>
-  <si>
-    <t>Umur Ekonomis (Tahun)</t>
-  </si>
-  <si>
-    <t>Nilai Perolehan</t>
-  </si>
-  <si>
-    <t>Merk</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Dept</t>
-  </si>
-  <si>
-    <t>Status</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>PIC</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -137,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -149,6 +137,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7210F671-66B7-488E-9E23-21BC8C84AFDD}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -483,11 +474,9 @@
     <col min="8" max="8" width="20.53515625" style="3" customWidth="1"/>
     <col min="9" max="9" width="20.3046875" style="4" customWidth="1"/>
     <col min="10" max="10" width="21.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="21.84375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.765625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,34 +490,27 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J3" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>